<commit_message>
Updated Model Research file
</commit_message>
<xml_diff>
--- a/Docs/Model_Research.xlsx
+++ b/Docs/Model_Research.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY LINGAMPALLI\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY LINGAMPALLI\OneDrive\Documents\GitHub\LanguageTranslationSystem\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ED734D-79AA-4020-8F78-DB20B99342FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30A9297-4643-4AC8-AE06-BD056A2D13D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5DF337A5-D9E2-47E4-B24D-BEA80230481B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Model Link</t>
   </si>
@@ -74,9 +74,6 @@
 Telugu (తెలుగు)
 Urdu (اردو)
 English</t>
-  </si>
-  <si>
-    <t>Required / CPU i7</t>
   </si>
   <si>
     <t>https://www.kaggle.com/models/google/muril/tensorFlow2/muril/1?tfhub-redirect=true</t>
@@ -108,9 +105,6 @@
   </si>
   <si>
     <t>Required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRI VARSAN N S </t>
   </si>
   <si>
     <t>Bengali (bn)
@@ -237,19 +231,115 @@
     <t>Samaksh ahuja</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>CPU Support ?</t>
+  </si>
+  <si>
+    <t>Multilingual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRI VARSAN N S 
+JESHTHA TAKTEWALE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nisha Verma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindi 
+Telugu 
+Marathi 
+Urdu
+Assamese 
+Konkani 
+Nepali
+Sindhi
+Tamil
+Kannada
+Malyalam 
+Gujarati 
+Punjabi 
+Bengali 
+Odia 
+English </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowed </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Required</t>
+  </si>
+  <si>
+    <t>Supports</t>
+  </si>
+  <si>
+    <t>Required for faster 
+inference</t>
+  </si>
+  <si>
+    <t>Harshavardan Bandari</t>
+  </si>
+  <si>
+    <t>Not  required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bengali
+English
+Gujarati
+Hindi
+Kannada
+Malayalam
+Marathi
+Sindhi
+Punjabi
+Tamil
+Telugu
+Urdu
+and other 95 foreign languages 
+</t>
+  </si>
+  <si>
+    <t>https://github.com/google-research/multilingual-t5</t>
+  </si>
+  <si>
+    <t>Supports
+i7/ ryzen 7</t>
+  </si>
+  <si>
+    <t>Supports
+i5/ryzen 5</t>
+  </si>
+  <si>
+    <t>Not strictly required </t>
+  </si>
+  <si>
+    <t>Amitabh</t>
+  </si>
+  <si>
+    <t>Bengali
+Gujarati
+Hindi
+Marathi
+Nepali
+Odia
+Tamil
+Telugu
+Sinhala
+Kannada (KB)
+Malayalam (KB)</t>
+  </si>
+  <si>
+    <t>Supports (i5 enough for distilled model)</t>
+  </si>
+  <si>
+    <t>https://github.com/AI4Bharat/IndicWav2Vec</t>
+  </si>
+  <si>
+    <t>Supports
+ i7/ryzen 7</t>
   </si>
   <si>
     <t>MAYALURI ANUSHA
-VIVEK LAKUM
 AJAY LINGAMPALLI
-HARSHAVARDAN BANDARI</t>
-  </si>
-  <si>
-    <t>CPU Support ?</t>
+VIVEK LAKUM</t>
   </si>
 </sst>
 </file>
@@ -289,7 +379,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -355,19 +445,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -395,20 +472,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -746,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792C460B-F1D9-44DA-B4A5-877BB70FE00E}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,206 +859,291 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>40</v>
+      <c r="G1" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2">
         <v>55</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2">
         <v>22</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>38</v>
+        <v>28</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="4">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="2">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2">
-        <v>10</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="4">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2">
-        <v>8</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2">
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="8"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
-    <sortCondition descending="1" ref="C1:C10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
+    <sortCondition descending="1" ref="C1:C13"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{C2A8F453-8FE5-48AA-9981-99A9C2FC4520}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{C2A8F453-8FE5-48AA-9981-99A9C2FC4520}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{11FEFE3F-5EF1-45F2-B24F-0F27FBCDAA1A}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{E01BF0AE-1C88-49FF-90F3-763F4B8963A0}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{E01BF0AE-1C88-49FF-90F3-763F4B8963A0}"/>
     <hyperlink ref="B3" r:id="rId4" xr:uid="{ED055DBB-67DE-41CE-8D75-1933EF5AB1DE}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{BCB282FA-6298-4047-8371-2DC589F8D079}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{47F56A40-2D48-4F4E-89E9-1DEF20B63CA9}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{BCB282FA-6298-4047-8371-2DC589F8D079}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{47F56A40-2D48-4F4E-89E9-1DEF20B63CA9}"/>
     <hyperlink ref="B2" r:id="rId7" xr:uid="{216D4E83-9C12-4E89-A890-23C1AFD0D471}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{938B128D-1DD8-4D7A-8D0A-3FFE896A2F8B}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{4274FE8C-5B9B-4041-9EFE-2B2CB71E9604}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{938B128D-1DD8-4D7A-8D0A-3FFE896A2F8B}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{4274FE8C-5B9B-4041-9EFE-2B2CB71E9604}"/>
+    <hyperlink ref="B5" r:id="rId10" xr:uid="{48A60184-E63C-4D93-A53B-9272625ACE56}"/>
+    <hyperlink ref="B7" r:id="rId11" xr:uid="{5B8CA96D-FE9F-47DD-983B-C469AC2F4A18}"/>
+    <hyperlink ref="B9" r:id="rId12" xr:uid="{B3B0ADD1-DC63-4D9A-8D8D-AA8F732B82E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>